<commit_message>
added new eng field
</commit_message>
<xml_diff>
--- a/others/domande.xlsx
+++ b/others/domande.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labateal\Desktop\exers\GUIDA\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9CABB6DF-858A-4FFC-A00F-C32EBCC0D93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{83FFCE6A-13FE-465B-8597-91BDE8E87428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29040" yWindow="2085" windowWidth="17280" windowHeight="9075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="domande" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="295" uniqueCount="238">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="578" uniqueCount="247">
   <si>
     <t>id_domande</t>
   </si>
@@ -750,13 +750,40 @@
   </si>
   <si>
     <t>I veicoli fuoristrada presentano un‘altezza tale da permettere al conducente una adeguata visibilità di tutti i possibili ostacoli in basso (ad esempio, bambini)</t>
+  </si>
+  <si>
+    <t>La patente di categoria BE abilita anche alla guida dei veicoli che si possono condurre con le patenti di categoria AM, B1, B e B con codice armonizzato 96</t>
+  </si>
+  <si>
+    <t>Nel caso in cui la sosta è espressamente vietata da una norma del codice della strada, l'osservanza di tale divieto è comunque condizionata dalla presenza di cartelli segnaletici</t>
+  </si>
+  <si>
+    <t>Il segnale raffigurato preannuncia incrocio con precedenza rispetto ai soli veicoli provenienti da destra</t>
+  </si>
+  <si>
+    <t>In presenza del segnale raffigurato è consentito il transito a tutti gli autosnodati per trasporto di persone</t>
+  </si>
+  <si>
+    <t>La patente di categoria A può essere conseguita, con accesso diretto, da chi non è già titolare di patente A2 da almeno 2 anni, solo se ha compiuto 24 anni di età</t>
+  </si>
+  <si>
+    <t>L'assicurazione obbligatoria RCA copre I danni subiti dai terzi trasportati se il veicolo è autorizzato al trasporto di persone</t>
+  </si>
+  <si>
+    <t>La spia di temperatura dell'acqua di raffreddamento è di colore rosso</t>
+  </si>
+  <si>
+    <t>testo_inglese</t>
+  </si>
+  <si>
+    <t>the stop is allowed at the exit of the driveaways</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -890,6 +917,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1233,8 +1265,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1590,18 +1625,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F241"/>
+  <dimension ref="A1:H248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="58.88671875" customWidth="1"/>
+    <col min="6" max="6" width="73.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1617,8 +1653,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1634,12 +1673,27 @@
       <c r="E2" t="s">
         <v>120</v>
       </c>
-      <c r="F2" t="str">
+      <c r="F2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" t="str">
         <f>_xlfn.CONCAT("INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (",A2,",'",B2,"',",C2,",",D2,",'",E2,"');")</f>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (1,'la fermata è consentita allo sbocco dei passi carrabili',0,0,'V');</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H2" s="1" t="str">
+        <f>_xlfn.CONCAT("{
+      question: '",B2,"',
+      choices: ['V', 'F'],
+      answer: '",E2,"'
+    },",)</f>
+        <v>{
+      question: 'la fermata è consentita allo sbocco dei passi carrabili',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1655,12 +1709,27 @@
       <c r="E3" t="s">
         <v>121</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F51" si="0">_xlfn.CONCAT("INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (",A3,",'",B3,"',",C3,",",D3,",'",E3,"');")</f>
+      <c r="F3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G67" si="0">_xlfn.CONCAT("INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (",A3,",'",B3,"',",C3,",",D3,",'",E3,"');")</f>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (2,'Nel caso in cui la sosta è espressamente vietata da una norma del codice stradale, l‘osservanza di tale divieto non è condizionata dalla presenza di cartelli segnaletici',0,0,'F');</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H3" s="1" t="str">
+        <f t="shared" ref="H3:H66" si="1">_xlfn.CONCAT("{
+      question: '",B3,"',
+      choices: ['V', 'F'],
+      answer: '",E3,"'
+    },",)</f>
+        <v>{
+      question: 'Nel caso in cui la sosta è espressamente vietata da una norma del codice stradale, l‘osservanza di tale divieto non è condizionata dalla presenza di cartelli segnaletici',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1676,12 +1745,23 @@
       <c r="E4" t="s">
         <v>121</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (3,' In caso di sosta in un centro abitato, il conducente deve collocare il veicolo il più vicino possibile al margine destro della carreggiata, anche dove non esiste il marciapiede rialzato',0,0,'F');</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: ' In caso di sosta in un centro abitato, il conducente deve collocare il veicolo il più vicino possibile al margine destro della carreggiata, anche dove non esiste il marciapiede rialzato',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1697,12 +1777,23 @@
       <c r="E5" t="s">
         <v>121</v>
       </c>
-      <c r="F5" t="str">
+      <c r="F5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (4,'Nel caso in cui la sosta è espressamente vietata da una norma del codice della strada, l‘osservanza di tale divieto è comunque condizionata dalla presenza di cartelli segnaletici',0,0,'F');</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Nel caso in cui la sosta è espressamente vietata da una norma del codice della strada, l‘osservanza di tale divieto è comunque condizionata dalla presenza di cartelli segnaletici',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1718,12 +1809,23 @@
       <c r="E6" t="s">
         <v>120</v>
       </c>
-      <c r="F6" t="str">
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (5,'La sosta e la fermata sono sempre vietate sugli attraversamenti pedonali',0,0,'V');</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'La sosta e la fermata sono sempre vietate sugli attraversamenti pedonali',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1739,12 +1841,23 @@
       <c r="E7" t="s">
         <v>120</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (6,'Su strade extraurbane principali il limite massimo di velocità è di 70 km/h per autovettura che traina caravan da 900 chilogrammi',0,0,'V');</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Su strade extraurbane principali il limite massimo di velocità è di 70 km/h per autovettura che traina caravan da 900 chilogrammi',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1760,12 +1873,23 @@
       <c r="E8" t="s">
         <v>120</v>
       </c>
-      <c r="F8" t="str">
+      <c r="F8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (7,'Sulla distanza di sicurezza influisce l‘efficienza del freno di servizio',0,0,'V');</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Sulla distanza di sicurezza influisce l‘efficienza del freno di servizio',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1781,12 +1905,23 @@
       <c r="E9" t="s">
         <v>121</v>
       </c>
-      <c r="F9" t="str">
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (8,'Il cono si usa per indicare un parcheggio riservato',0,0,'F');</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il cono si usa per indicare un parcheggio riservato',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1802,12 +1937,23 @@
       <c r="E10" t="s">
         <v>120</v>
       </c>
-      <c r="F10" t="str">
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (9,'La sosta e la fermata sono vietate in corrispondenza dei segnali orizzontali di preselezione e lungo le corsie di canalizzazione',0,0,'V');</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'La sosta e la fermata sono vietate in corrispondenza dei segnali orizzontali di preselezione e lungo le corsie di canalizzazione',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1823,12 +1969,23 @@
       <c r="E11" t="s">
         <v>120</v>
       </c>
-      <c r="F11" t="str">
+      <c r="F11" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (10,'È consentito il sorpasso in prossimità o in corrispondenza di passaggi a livello senza barriere se la circolazione è regolata da semafori',0,0,'V');</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'È consentito il sorpasso in prossimità o in corrispondenza di passaggi a livello senza barriere se la circolazione è regolata da semafori',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1844,12 +2001,23 @@
       <c r="E12" t="s">
         <v>120</v>
       </c>
-      <c r="F12" t="str">
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (11,'I motocicli con cilindrata di almeno 150 cm3 possono circolare in autostrada',0,0,'V');</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'I motocicli con cilindrata di almeno 150 cm3 possono circolare in autostrada',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1865,12 +2033,23 @@
       <c r="E13" t="s">
         <v>120</v>
       </c>
-      <c r="F13" t="str">
+      <c r="F13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (12,'L‘attraversamento pedonale è una parte della carreggiata sulla quale è vietata la fermata dei veicoli',0,0,'V');</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'L‘attraversamento pedonale è una parte della carreggiata sulla quale è vietata la fermata dei veicoli',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1886,12 +2065,23 @@
       <c r="E14" t="s">
         <v>120</v>
       </c>
-      <c r="F14" t="str">
+      <c r="F14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (13,'Quando la carreggiata extraurbana è occupata da ciclisti o pedoni, è consigliabile suonare il clacson prima di sorpassarli',0,0,'V');</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Quando la carreggiata extraurbana è occupata da ciclisti o pedoni, è consigliabile suonare il clacson prima di sorpassarli',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1907,12 +2097,23 @@
       <c r="E15" t="s">
         <v>121</v>
       </c>
-      <c r="F15" t="str">
+      <c r="F15" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (14,'L‘isola di traffico è una zona destinata al parcheggio dei veicoli',0,0,'F');</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'L‘isola di traffico è una zona destinata al parcheggio dei veicoli',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1928,12 +2129,23 @@
       <c r="E16" t="s">
         <v>121</v>
       </c>
-      <c r="F16" t="str">
+      <c r="F16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (15,'Il marciapiede è una parte della strada dove, di norma, è consentita la sosta dei ciclomotori',0,0,'F');</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il marciapiede è una parte della strada dove, di norma, è consentita la sosta dei ciclomotori',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1949,12 +2161,23 @@
       <c r="E17" t="s">
         <v>121</v>
       </c>
-      <c r="F17" t="str">
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (16,'Si definiscono ciclomotori tutti i veicoli a due ruote di cilindrata superiore a 50 cm3',0,0,'F');</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Si definiscono ciclomotori tutti i veicoli a due ruote di cilindrata superiore a 50 cm3',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1970,12 +2193,23 @@
       <c r="E18" t="s">
         <v>120</v>
       </c>
-      <c r="F18" t="str">
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (17,'La carreggiata non comprende la pista ciclabile',0,0,'V');</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'La carreggiata non comprende la pista ciclabile',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1991,12 +2225,23 @@
       <c r="E19" t="s">
         <v>121</v>
       </c>
-      <c r="F19" t="str">
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (18,'La corsia di decelerazione serve per entrare in una piazzola di sosta',0,0,'F');</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'La corsia di decelerazione serve per entrare in una piazzola di sosta',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2012,12 +2257,23 @@
       <c r="E20" t="s">
         <v>121</v>
       </c>
-      <c r="F20" t="str">
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (19,'Fanno parte della carreggiata le corsie di emergenza delle autostrade',0,0,'F');</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Fanno parte della carreggiata le corsie di emergenza delle autostrade',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2033,12 +2289,23 @@
       <c r="E21" t="s">
         <v>120</v>
       </c>
-      <c r="F21" t="str">
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (20,'I ciclomotori a due ruote non possono avere un motore termico di clindrata superiore a 50 cm3',0,0,'V');</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'I ciclomotori a due ruote non possono avere un motore termico di clindrata superiore a 50 cm3',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2054,12 +2321,23 @@
       <c r="E22" t="s">
         <v>120</v>
       </c>
-      <c r="F22" t="str">
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (21,'I tricicli a motore sono veicoli con motore di cilindrata superiore a 50 cm3',0,0,'V');</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'I tricicli a motore sono veicoli con motore di cilindrata superiore a 50 cm3',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2075,12 +2353,23 @@
       <c r="E23" t="s">
         <v>120</v>
       </c>
-      <c r="F23" t="str">
+      <c r="F23" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (22,'I montanti interni degli autoveicoli condizionano la visibilità',0,0,'V');</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'I montanti interni degli autoveicoli condizionano la visibilità',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2096,12 +2385,23 @@
       <c r="E24" t="s">
         <v>121</v>
       </c>
-      <c r="F24" t="str">
+      <c r="F24" t="s">
+        <v>128</v>
+      </c>
+      <c r="G24" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (23,'Le strade extraurbane principali possono essere ad un‘unica carreggiata',0,0,'F');</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Le strade extraurbane principali possono essere ad un‘unica carreggiata',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2117,12 +2417,23 @@
       <c r="E25" t="s">
         <v>120</v>
       </c>
-      <c r="F25" t="str">
+      <c r="F25" t="s">
+        <v>129</v>
+      </c>
+      <c r="G25" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (24,'L‘autocaravan non è un rimorchio ',0,0,'V');</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'L‘autocaravan non è un rimorchio ',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2138,12 +2449,23 @@
       <c r="E26" t="s">
         <v>121</v>
       </c>
-      <c r="F26" t="str">
+      <c r="F26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (25,'Fuori dai centri abitati, su una stessa corsia possono circolare affiancati due ciclomotiri',0,0,'F');</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Fuori dai centri abitati, su una stessa corsia possono circolare affiancati due ciclomotiri',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2159,12 +2481,23 @@
       <c r="E27" t="s">
         <v>121</v>
       </c>
-      <c r="F27" t="str">
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (26,'Le biciclette con pedala assistita, dotate di motore elettrico ausiliario di potenza massima fino a 0,25 kw, sono definite ciclomotori',0,0,'F');</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Le biciclette con pedala assistita, dotate di motore elettrico ausiliario di potenza massima fino a 0,25 kw, sono definite ciclomotori',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2180,12 +2513,23 @@
       <c r="E28" t="s">
         <v>121</v>
       </c>
-      <c r="F28" t="str">
+      <c r="F28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (27,'Il passaggio a livello è un passo carrabile ',0,0,'F');</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il passaggio a livello è un passo carrabile ',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2201,12 +2545,23 @@
       <c r="E29" t="s">
         <v>121</v>
       </c>
-      <c r="F29" t="str">
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (28,'Fanno parte della carreggiata le corsie di emergenza delle autostrade',0,0,'F');</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Fanno parte della carreggiata le corsie di emergenza delle autostrade',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2222,12 +2577,23 @@
       <c r="E30" t="s">
         <v>121</v>
       </c>
-      <c r="F30" t="str">
+      <c r="F30" t="s">
+        <v>110</v>
+      </c>
+      <c r="G30" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (29,'Su una strada ricoperta da brecciolino il conducente può circolare a velocità sostenuta',0,0,'F');</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Su una strada ricoperta da brecciolino il conducente può circolare a velocità sostenuta',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2243,12 +2609,23 @@
       <c r="E31" t="s">
         <v>121</v>
       </c>
-      <c r="F31" t="str">
+      <c r="F31" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (30,'La corsia può essere a doppio senso di circolazione',0,0,'F');</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H31" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'La corsia può essere a doppio senso di circolazione',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2264,12 +2641,23 @@
       <c r="E32" t="s">
         <v>121</v>
       </c>
-      <c r="F32" t="str">
+      <c r="F32" t="s">
+        <v>130</v>
+      </c>
+      <c r="G32" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (31,'L‘attraversamento pedonale è una parte della carreggiata vietata al transito dei veicoli',0,0,'F');</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'L‘attraversamento pedonale è una parte della carreggiata vietata al transito dei veicoli',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2285,12 +2673,23 @@
       <c r="E33" t="s">
         <v>120</v>
       </c>
-      <c r="F33" t="str">
+      <c r="F33" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (32,'Nelle aree pedonali possono transitare gli autoveicoli dei vigili del fuoco con luce lampeggiante blu e sirena in funzione',0,0,'V');</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Nelle aree pedonali possono transitare gli autoveicoli dei vigili del fuoco con luce lampeggiante blu e sirena in funzione',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2306,12 +2705,23 @@
       <c r="E34" t="s">
         <v>121</v>
       </c>
-      <c r="F34" t="str">
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (33,'I quadricicli non leggeri, ai fini della circolazione, sono equiparati ai ciclomotori',0,0,'F');</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'I quadricicli non leggeri, ai fini della circolazione, sono equiparati ai ciclomotori',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2327,12 +2737,23 @@
       <c r="E35" t="s">
         <v>121</v>
       </c>
-      <c r="F35" t="str">
+      <c r="F35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (34,'Durante la circolazione, gli autocarri di massa complessiva a pieno carico inferiore o uguale a 3,5 tonnellate devono essere segnalati posteriormente con pannelli retroriflettenti gialli e rossi',0,0,'F');</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H35" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Durante la circolazione, gli autocarri di massa complessiva a pieno carico inferiore o uguale a 3,5 tonnellate devono essere segnalati posteriormente con pannelli retroriflettenti gialli e rossi',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2348,12 +2769,23 @@
       <c r="E36" t="s">
         <v>121</v>
       </c>
-      <c r="F36" t="str">
+      <c r="F36" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (35,'Bisogna usare particolare prudenza nei confronti dei conducenti che hanno conseguito la patente di guida in uno stato estero',0,0,'F');</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Bisogna usare particolare prudenza nei confronti dei conducenti che hanno conseguito la patente di guida in uno stato estero',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2369,12 +2801,23 @@
       <c r="E37" t="s">
         <v>121</v>
       </c>
-      <c r="F37" t="str">
+      <c r="F37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G37" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (36,'Sulle strade extraurbane principali è consentito circolare alla velocità massima di 130 km/h',0,0,'F');</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H37" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Sulle strade extraurbane principali è consentito circolare alla velocità massima di 130 km/h',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2390,12 +2833,23 @@
       <c r="E38" t="s">
         <v>121</v>
       </c>
-      <c r="F38" t="str">
+      <c r="F38" t="s">
+        <v>131</v>
+      </c>
+      <c r="G38" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (37,'L‘isola di traffico serve per il transito dei pedoni',0,0,'F');</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H38" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'L‘isola di traffico serve per il transito dei pedoni',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2411,12 +2865,23 @@
       <c r="E39" t="s">
         <v>121</v>
       </c>
-      <c r="F39" t="str">
+      <c r="F39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (38,'Si definisce autovettura il veicolo blindato e attrezzato per il trasporto di valori',0,0,'F');</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H39" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Si definisce autovettura il veicolo blindato e attrezzato per il trasporto di valori',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2432,12 +2897,23 @@
       <c r="E40" t="s">
         <v>121</v>
       </c>
-      <c r="F40" t="str">
+      <c r="F40" t="s">
+        <v>90</v>
+      </c>
+      <c r="G40" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (39,'Il passaggio a livello è un cavalcavia ferroviario o tranviario',0,0,'F');</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H40" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il passaggio a livello è un cavalcavia ferroviario o tranviario',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2453,12 +2929,23 @@
       <c r="E41" t="s">
         <v>121</v>
       </c>
-      <c r="F41" t="str">
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (40,'Con la patente di categoria A si possono guidare tutte le macchine agricole',0,0,'F');</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H41" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Con la patente di categoria A si possono guidare tutte le macchine agricole',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2474,12 +2961,23 @@
       <c r="E42" t="s">
         <v>121</v>
       </c>
-      <c r="F42" t="str">
+      <c r="F42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (41,'Bisogna lasciare liberi gli ingressi delle abitazioni private in caso di formazione di code di veicoli',0,0,'F');</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H42" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Bisogna lasciare liberi gli ingressi delle abitazioni private in caso di formazione di code di veicoli',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2495,12 +2993,23 @@
       <c r="E43" t="s">
         <v>121</v>
       </c>
-      <c r="F43" t="str">
+      <c r="F43" t="s">
+        <v>91</v>
+      </c>
+      <c r="G43" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (42,'Il passaggio a livello è caratterizzato dalla presenza di un attraversamento autostradale',0,0,'F');</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H43" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il passaggio a livello è caratterizzato dalla presenza di un attraversamento autostradale',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2516,12 +3025,23 @@
       <c r="E44" t="s">
         <v>120</v>
       </c>
-      <c r="F44" t="str">
+      <c r="F44" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (43,'Quando vi sono bambini fermi al semaforo bisogna usare prudenza, perchè‚ potrebbero scendere dal marciapiede, invadendo la carreggiata, quando ancora per loro il semaforo è disposto al rosso',0,0,'V');</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H44" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Quando vi sono bambini fermi al semaforo bisogna usare prudenza, perchè‚ potrebbero scendere dal marciapiede, invadendo la carreggiata, quando ancora per loro il semaforo è disposto al rosso',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2537,12 +3057,23 @@
       <c r="E45" t="s">
         <v>120</v>
       </c>
-      <c r="F45" t="str">
+      <c r="F45" t="s">
+        <v>132</v>
+      </c>
+      <c r="G45" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (44,'L‘autostrada non ha incroci a raso che l‘attraversano',0,0,'V');</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H45" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'L‘autostrada non ha incroci a raso che l‘attraversano',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2558,12 +3089,23 @@
       <c r="E46" t="s">
         <v>121</v>
       </c>
-      <c r="F46" t="str">
+      <c r="F46" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (45,'La corsia di accelerazione serve per uscire da una piazzola di sosta',0,0,'F');</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H46" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'La corsia di accelerazione serve per uscire da una piazzola di sosta',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2579,12 +3121,23 @@
       <c r="E47" t="s">
         <v>121</v>
       </c>
-      <c r="F47" t="str">
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (46,'Fanno parte della carreggiata le corsie di emergenza delle autostrade',0,0,'F');</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H47" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Fanno parte della carreggiata le corsie di emergenza delle autostrade',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2600,12 +3153,23 @@
       <c r="E48" t="s">
         <v>121</v>
       </c>
-      <c r="F48" t="str">
+      <c r="F48" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (47,'Bisogna lasciare liberi i sottovia in caso di traffico intenso',0,0,'F');</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H48" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Bisogna lasciare liberi i sottovia in caso di traffico intenso',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2621,12 +3185,23 @@
       <c r="E49" t="s">
         <v>121</v>
       </c>
-      <c r="F49" t="str">
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (48,'Avvicinandosi ad un passaggio a livello con luci rosse accese e semibarriera ancora alzata, bisogna fermarsi in corrispondenza del terzo pannello distanziometrico',0,0,'F');</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H49" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Avvicinandosi ad un passaggio a livello con luci rosse accese e semibarriera ancora alzata, bisogna fermarsi in corrispondenza del terzo pannello distanziometrico',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2642,12 +3217,23 @@
       <c r="E50" t="s">
         <v>121</v>
       </c>
-      <c r="F50" t="str">
+      <c r="F50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (49,'Il conducente che intende sorpassare ciclisti o pedoni che occupano la carreggiata deve mantenere una distanza laterale di almeno 2 metri',0,0,'F');</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H50" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il conducente che intende sorpassare ciclisti o pedoni che occupano la carreggiata deve mantenere una distanza laterale di almeno 2 metri',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2663,12 +3249,23 @@
       <c r="E51" t="s">
         <v>121</v>
       </c>
-      <c r="F51" t="str">
+      <c r="F51" t="s">
+        <v>153</v>
+      </c>
+      <c r="G51" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (50,'Per evitare rumori fastidiosi, occorre chiudere con forza le portiere in modo da non doverle richiudere',0,0,'F');</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H51" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Per evitare rumori fastidiosi, occorre chiudere con forza le portiere in modo da non doverle richiudere',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2681,8 +3278,26 @@
       <c r="D52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>121</v>
+      </c>
+      <c r="F52" t="s">
+        <v>133</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (51,'Per diminuire l‘inquinamento dell‘aria provocato dai veicoli, bisogna controllare spesso la frizione e il differenziale',0,0,'F');</v>
+      </c>
+      <c r="H52" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Per diminuire l‘inquinamento dell‘aria provocato dai veicoli, bisogna controllare spesso la frizione e il differenziale',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2695,8 +3310,26 @@
       <c r="D53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E53" t="s">
+        <v>120</v>
+      </c>
+      <c r="F53" t="s">
+        <v>154</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (52,'È consentito l‘uso intermittente dei proiettori profondità per segnalare al veicolo che precede, anche all‘interno dei centri abitati, l‘intenzione di sorpassare',0,0,'V');</v>
+      </c>
+      <c r="H53" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'È consentito l‘uso intermittente dei proiettori profondità per segnalare al veicolo che precede, anche all‘interno dei centri abitati, l‘intenzione di sorpassare',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2709,8 +3342,26 @@
       <c r="D54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
+        <v>120</v>
+      </c>
+      <c r="F54" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (53,'La luce gialla lampeggiante, del tipo C in figura, indica che svoltando a destra i veicoli devono dare la precedenza alle biciclette',0,1,'V');</v>
+      </c>
+      <c r="H54" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'La luce gialla lampeggiante, del tipo C in figura, indica che svoltando a destra i veicoli devono dare la precedenza alle biciclette',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2723,8 +3374,26 @@
       <c r="D55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E55" t="s">
+        <v>121</v>
+      </c>
+      <c r="F55" t="s">
+        <v>29</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (54,'Il vigile disposto con le braccia ad angolo retto come in figura consente di svoltare a destra ai veicoli che arrivano dalla sua destra',0,3,'F');</v>
+      </c>
+      <c r="H55" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il vigile disposto con le braccia ad angolo retto come in figura consente di svoltare a destra ai veicoli che arrivano dalla sua destra',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2737,8 +3406,26 @@
       <c r="D56">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E56" t="s">
+        <v>121</v>
+      </c>
+      <c r="F56" t="s">
+        <v>92</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (55,'Quando è accesa la luce verde del semaforo in figura, il conducente che svolta a sinistra ha la precedenza sui veicoli che provengono di fronte',0,5,'F');</v>
+      </c>
+      <c r="H56" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Quando è accesa la luce verde del semaforo in figura, il conducente che svolta a sinistra ha la precedenza sui veicoli che provengono di fronte',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2751,8 +3438,26 @@
       <c r="D57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E57" t="s">
+        <v>121</v>
+      </c>
+      <c r="F57" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (56,'La luce gialla lampeggiante, del tipo B in figura, indica la presenza di un viale pedonale',0,1,'F');</v>
+      </c>
+      <c r="H57" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'La luce gialla lampeggiante, del tipo B in figura, indica la presenza di un viale pedonale',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2765,8 +3470,26 @@
       <c r="D58">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E58" t="s">
+        <v>120</v>
+      </c>
+      <c r="F58" t="s">
+        <v>134</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (57,'Le luci rosse accese lampeggianti in figura obbligano ad arrestarsi all‘accesso di un pontile d‘imbarco di navi traghetto',0,2,'V');</v>
+      </c>
+      <c r="H58" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Le luci rosse accese lampeggianti in figura obbligano ad arrestarsi all‘accesso di un pontile d‘imbarco di navi traghetto',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2779,8 +3502,26 @@
       <c r="D59">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E59" t="s">
+        <v>121</v>
+      </c>
+      <c r="F59" t="s">
+        <v>135</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (58,'Il segnale raffigurato indica che nelle vicinanze vi è un‘area di sosta per autoveicoli',0,9,'F');</v>
+      </c>
+      <c r="H59" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il segnale raffigurato indica che nelle vicinanze vi è un‘area di sosta per autoveicoli',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2793,8 +3534,26 @@
       <c r="D60">
         <v>11</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E60" t="s">
+        <v>120</v>
+      </c>
+      <c r="F60" t="s">
+        <v>31</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (59,'Il segnale raffigurato consente la svolta a destra ',0,11,'V');</v>
+      </c>
+      <c r="H60" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il segnale raffigurato consente la svolta a destra ',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2807,8 +3566,26 @@
       <c r="D61">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E61" t="s">
+        <v>120</v>
+      </c>
+      <c r="F61" t="s">
+        <v>32</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (60,'Il segnale raffigurato, se posto sul bordo del marciapiede, indica la fermata di uno scuolabus ',0,10,'V');</v>
+      </c>
+      <c r="H61" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il segnale raffigurato, se posto sul bordo del marciapiede, indica la fermata di uno scuolabus ',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2821,8 +3598,26 @@
       <c r="D62">
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E62" t="s">
+        <v>121</v>
+      </c>
+      <c r="F62" t="s">
+        <v>136</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (61,'Il segnale raffigurato si trova all‘ingresso di un‘autostrada',0,8,'F');</v>
+      </c>
+      <c r="H62" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il segnale raffigurato si trova all‘ingresso di un‘autostrada',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2835,8 +3630,26 @@
       <c r="D63">
         <v>7</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E63" t="s">
+        <v>121</v>
+      </c>
+      <c r="F63" t="s">
+        <v>93</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (62,'Il semaforo in figura è valido solo per i veicoli che marciano su rotaie (tram, treni)',0,7,'F');</v>
+      </c>
+      <c r="H63" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il semaforo in figura è valido solo per i veicoli che marciano su rotaie (tram, treni)',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2849,8 +3662,26 @@
       <c r="D64">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E64" t="s">
+        <v>120</v>
+      </c>
+      <c r="F64" t="s">
+        <v>103</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (63,'Quando il vigile si dispone di profilo con le braccia aperte come in figura si può svoltare a destra se si proviene dalla sua destra o dalla sua sinistra',0,3,'V');</v>
+      </c>
+      <c r="H64" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Quando il vigile si dispone di profilo con le braccia aperte come in figura si può svoltare a destra se si proviene dalla sua destra o dalla sua sinistra',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2863,8 +3694,26 @@
       <c r="D65">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E65" t="s">
+        <v>120</v>
+      </c>
+      <c r="F65" t="s">
+        <v>33</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (64,'Il vigile disposto con le braccia ad angolo retto come in figura consente di proseguire diritto ai veicoli che arrivano dalla sua sinistra',0,4,'V');</v>
+      </c>
+      <c r="H65" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il vigile disposto con le braccia ad angolo retto come in figura consente di proseguire diritto ai veicoli che arrivano dalla sua sinistra',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2877,8 +3726,26 @@
       <c r="D66">
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E66" t="s">
+        <v>121</v>
+      </c>
+      <c r="F66" t="s">
+        <v>34</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (65,'Il semaforo di corsie reversibili in figura indica la corsia per la sosta di emergenza ',0,6,'F');</v>
+      </c>
+      <c r="H66" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>{
+      question: 'Il semaforo di corsie reversibili in figura indica la corsia per la sosta di emergenza ',
+      choices: ['V', 'F'],
+      answer: 'F'
+    },</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2891,8 +3758,30 @@
       <c r="D67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E67" t="s">
+        <v>120</v>
+      </c>
+      <c r="F67" t="s">
+        <v>35</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO domande(id_domanda, testo, id_categoria, id_immagine, risposta) VALUES (66,'Chi guida autoveicoli deve esibire, a richiesta degli agenti, il segnale mobile di pericolo (triangolo)',0,0,'V');</v>
+      </c>
+      <c r="H67" s="1" t="str">
+        <f t="shared" ref="H67" si="2">_xlfn.CONCAT("{
+      question: '",B67,"',
+      choices: ['V', 'F'],
+      answer: '",E67,"'
+    },",)</f>
+        <v>{
+      question: 'Chi guida autoveicoli deve esibire, a richiesta degli agenti, il segnale mobile di pericolo (triangolo)',
+      choices: ['V', 'F'],
+      answer: 'V'
+    },</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2905,8 +3794,11 @@
       <c r="D68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F68" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2919,8 +3811,11 @@
       <c r="D69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F69" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2933,8 +3828,11 @@
       <c r="D70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F70" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2947,8 +3845,11 @@
       <c r="D71">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F71" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2961,8 +3862,11 @@
       <c r="D72">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F72" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2975,8 +3879,11 @@
       <c r="D73">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F73" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2989,8 +3896,11 @@
       <c r="D74">
         <v>14</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F74" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3003,8 +3913,11 @@
       <c r="D75">
         <v>15</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F75" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3017,8 +3930,11 @@
       <c r="D76">
         <v>16</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F76" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3031,8 +3947,11 @@
       <c r="D77">
         <v>17</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F77" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3045,8 +3964,11 @@
       <c r="D78">
         <v>18</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F78" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3059,8 +3981,11 @@
       <c r="D79">
         <v>19</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F79" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3073,8 +3998,11 @@
       <c r="D80">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F80" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3087,8 +4015,11 @@
       <c r="D81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F81" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3101,8 +4032,11 @@
       <c r="D82">
         <v>20</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F82" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3115,8 +4049,11 @@
       <c r="D83">
         <v>21</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F83" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3129,8 +4066,11 @@
       <c r="D84">
         <v>22</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F84" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3143,8 +4083,11 @@
       <c r="D85">
         <v>23</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F85" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3157,8 +4100,11 @@
       <c r="D86">
         <v>24</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F86" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3171,8 +4117,11 @@
       <c r="D87">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F87" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3185,8 +4134,11 @@
       <c r="D88">
         <v>25</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F88" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3199,8 +4151,11 @@
       <c r="D89">
         <v>26</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F89" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3213,8 +4168,11 @@
       <c r="D90">
         <v>27</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F90" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3227,8 +4185,11 @@
       <c r="D91">
         <v>28</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F91" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3241,8 +4202,11 @@
       <c r="D92">
         <v>29</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F92" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3255,8 +4219,11 @@
       <c r="D93">
         <v>23</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F93" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3269,8 +4236,11 @@
       <c r="D94">
         <v>22</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F94" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3283,8 +4253,11 @@
       <c r="D95">
         <v>30</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F95" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3297,8 +4270,11 @@
       <c r="D96">
         <v>31</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F96" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3311,8 +4287,11 @@
       <c r="D97">
         <v>31</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F97" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3325,8 +4304,11 @@
       <c r="D98">
         <v>32</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F98" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3339,8 +4321,11 @@
       <c r="D99">
         <v>33</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F99" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3353,8 +4338,11 @@
       <c r="D100">
         <v>34</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F100" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3367,8 +4355,11 @@
       <c r="D101">
         <v>35</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F101" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3381,8 +4372,11 @@
       <c r="D102">
         <v>36</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F102" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3395,8 +4389,11 @@
       <c r="D103">
         <v>37</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F103" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3409,8 +4406,11 @@
       <c r="D104">
         <v>38</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F104" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3423,8 +4423,11 @@
       <c r="D105">
         <v>39</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F105" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3437,8 +4440,11 @@
       <c r="D106">
         <v>40</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F106" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3451,8 +4457,11 @@
       <c r="D107">
         <v>39</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F107" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3465,8 +4474,11 @@
       <c r="D108">
         <v>13</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F108" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3479,8 +4491,11 @@
       <c r="D109">
         <v>14</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F109" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3493,8 +4508,11 @@
       <c r="D110">
         <v>41</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F110" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3507,8 +4525,11 @@
       <c r="D111">
         <v>42</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F111" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3521,8 +4542,11 @@
       <c r="D112">
         <v>43</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F112" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3535,8 +4559,11 @@
       <c r="D113">
         <v>44</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F113" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3549,8 +4576,11 @@
       <c r="D114">
         <v>42</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F114" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3563,8 +4593,11 @@
       <c r="D115">
         <v>45</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F115" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3577,8 +4610,11 @@
       <c r="D116">
         <v>46</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F116" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3591,8 +4627,11 @@
       <c r="D117">
         <v>47</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F117" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3605,8 +4644,11 @@
       <c r="D118">
         <v>48</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F118" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3619,8 +4661,11 @@
       <c r="D119">
         <v>49</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F119" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3633,8 +4678,11 @@
       <c r="D120">
         <v>49</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F120" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3647,8 +4695,11 @@
       <c r="D121">
         <v>50</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F121" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3661,8 +4712,11 @@
       <c r="D122">
         <v>51</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F122" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -3675,8 +4729,11 @@
       <c r="D123">
         <v>52</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F123" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -3689,8 +4746,11 @@
       <c r="D124">
         <v>53</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F124" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -3703,8 +4763,11 @@
       <c r="D125">
         <v>54</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F125" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -3717,8 +4780,11 @@
       <c r="D126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F126" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3731,8 +4797,11 @@
       <c r="D127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F127" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3745,8 +4814,11 @@
       <c r="D128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F128" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3759,8 +4831,11 @@
       <c r="D129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F129" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3773,8 +4848,11 @@
       <c r="D130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F130" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3787,8 +4865,11 @@
       <c r="D131">
         <v>42</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F131" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -3801,8 +4882,11 @@
       <c r="D132">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F132" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -3815,8 +4899,11 @@
       <c r="D133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F133" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -3829,8 +4916,11 @@
       <c r="D134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F134" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -3843,8 +4933,11 @@
       <c r="D135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F135" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -3857,8 +4950,11 @@
       <c r="D136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F136" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -3871,8 +4967,11 @@
       <c r="D137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F137" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -3885,8 +4984,11 @@
       <c r="D138">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F138" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -3899,8 +5001,11 @@
       <c r="D139">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F139" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -3913,8 +5018,11 @@
       <c r="D140">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F140" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -3927,8 +5035,11 @@
       <c r="D141">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F141" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -3941,8 +5052,11 @@
       <c r="D142">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F142" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -3955,8 +5069,11 @@
       <c r="D143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F143" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -3969,8 +5086,11 @@
       <c r="D144">
         <v>55</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F144" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
@@ -3983,8 +5103,11 @@
       <c r="D145">
         <v>56</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F145" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
@@ -3997,8 +5120,11 @@
       <c r="D146">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F146" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>146</v>
       </c>
@@ -4011,8 +5137,11 @@
       <c r="D147">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F147" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>147</v>
       </c>
@@ -4025,8 +5154,11 @@
       <c r="D148">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F148" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>148</v>
       </c>
@@ -4039,8 +5171,11 @@
       <c r="D149">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F149" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>149</v>
       </c>
@@ -4053,8 +5188,11 @@
       <c r="D150">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F150" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
@@ -4067,8 +5205,11 @@
       <c r="D151">
         <v>28</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F151" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>151</v>
       </c>
@@ -4081,8 +5222,11 @@
       <c r="D152">
         <v>57</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F152" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>152</v>
       </c>
@@ -4095,8 +5239,11 @@
       <c r="D153">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F153" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>153</v>
       </c>
@@ -4109,8 +5256,11 @@
       <c r="D154">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F154" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>154</v>
       </c>
@@ -4123,8 +5273,11 @@
       <c r="D155">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F155" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>155</v>
       </c>
@@ -4137,8 +5290,11 @@
       <c r="D156">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F156" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>156</v>
       </c>
@@ -4151,8 +5307,11 @@
       <c r="D157">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F157" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>157</v>
       </c>
@@ -4165,8 +5324,11 @@
       <c r="D158">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F158" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>158</v>
       </c>
@@ -4179,8 +5341,11 @@
       <c r="D159">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F159" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>159</v>
       </c>
@@ -4193,8 +5358,11 @@
       <c r="D160">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F160" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
@@ -4207,8 +5375,11 @@
       <c r="D161">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F161" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
@@ -4221,8 +5392,11 @@
       <c r="D162">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F162" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
@@ -4235,8 +5409,11 @@
       <c r="D163">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F163" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
@@ -4249,8 +5426,11 @@
       <c r="D164">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F164" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
@@ -4263,8 +5443,11 @@
       <c r="D165">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F165" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
@@ -4277,8 +5460,11 @@
       <c r="D166">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F166" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
@@ -4291,8 +5477,11 @@
       <c r="D167">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F167" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
@@ -4305,8 +5494,11 @@
       <c r="D168">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F168" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
@@ -4319,8 +5511,11 @@
       <c r="D169">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F169" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
@@ -4333,8 +5528,11 @@
       <c r="D170">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F170" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
@@ -4347,8 +5545,11 @@
       <c r="D171">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F171" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
@@ -4361,8 +5562,11 @@
       <c r="D172">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F172" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
@@ -4375,8 +5579,11 @@
       <c r="D173">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F173" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
@@ -4389,8 +5596,11 @@
       <c r="D174">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F174" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>174</v>
       </c>
@@ -4403,8 +5613,11 @@
       <c r="D175">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F175" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>175</v>
       </c>
@@ -4417,8 +5630,11 @@
       <c r="D176">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F176" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>176</v>
       </c>
@@ -4431,8 +5647,11 @@
       <c r="D177">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F177" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>177</v>
       </c>
@@ -4445,8 +5664,11 @@
       <c r="D178">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F178" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>178</v>
       </c>
@@ -4459,8 +5681,11 @@
       <c r="D179">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F179" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>179</v>
       </c>
@@ -4473,8 +5698,11 @@
       <c r="D180">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F180" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>180</v>
       </c>
@@ -4487,8 +5715,11 @@
       <c r="D181">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F181" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>181</v>
       </c>
@@ -4501,8 +5732,11 @@
       <c r="D182">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F182" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>182</v>
       </c>
@@ -4515,8 +5749,11 @@
       <c r="D183">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F183" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>183</v>
       </c>
@@ -4529,8 +5766,11 @@
       <c r="D184">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F184" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>184</v>
       </c>
@@ -4543,8 +5783,11 @@
       <c r="D185">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F185" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>185</v>
       </c>
@@ -4557,8 +5800,11 @@
       <c r="D186">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F186" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>186</v>
       </c>
@@ -4571,8 +5817,11 @@
       <c r="D187">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F187" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>187</v>
       </c>
@@ -4585,8 +5834,11 @@
       <c r="D188">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F188" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>188</v>
       </c>
@@ -4599,8 +5851,11 @@
       <c r="D189">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F189" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>189</v>
       </c>
@@ -4613,8 +5868,11 @@
       <c r="D190">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F190" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>190</v>
       </c>
@@ -4627,8 +5885,11 @@
       <c r="D191">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F191" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>191</v>
       </c>
@@ -4641,8 +5902,11 @@
       <c r="D192">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F192" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>192</v>
       </c>
@@ -4655,8 +5919,11 @@
       <c r="D193">
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F193" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>193</v>
       </c>
@@ -4669,8 +5936,11 @@
       <c r="D194">
         <v>0</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F194" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>194</v>
       </c>
@@ -4683,8 +5953,11 @@
       <c r="D195">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F195" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>195</v>
       </c>
@@ -4697,8 +5970,11 @@
       <c r="D196">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F196" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>196</v>
       </c>
@@ -4711,8 +5987,11 @@
       <c r="D197">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F197" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>197</v>
       </c>
@@ -4725,8 +6004,11 @@
       <c r="D198">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F198" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>198</v>
       </c>
@@ -4739,8 +6021,11 @@
       <c r="D199">
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F199" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>199</v>
       </c>
@@ -4753,8 +6038,11 @@
       <c r="D200">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F200" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>200</v>
       </c>
@@ -4767,8 +6055,11 @@
       <c r="D201">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F201" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>201</v>
       </c>
@@ -4781,8 +6072,11 @@
       <c r="D202">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F202" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>202</v>
       </c>
@@ -4795,8 +6089,11 @@
       <c r="D203">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F203" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>203</v>
       </c>
@@ -4809,8 +6106,11 @@
       <c r="D204">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F204" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>204</v>
       </c>
@@ -4823,8 +6123,11 @@
       <c r="D205">
         <v>0</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F205" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>205</v>
       </c>
@@ -4837,8 +6140,11 @@
       <c r="D206">
         <v>0</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F206" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>206</v>
       </c>
@@ -4851,8 +6157,11 @@
       <c r="D207">
         <v>0</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F207" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>207</v>
       </c>
@@ -4865,8 +6174,11 @@
       <c r="D208">
         <v>0</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F208" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>208</v>
       </c>
@@ -4879,8 +6191,11 @@
       <c r="D209">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F209" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>209</v>
       </c>
@@ -4893,8 +6208,11 @@
       <c r="D210">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F210" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>210</v>
       </c>
@@ -4907,8 +6225,11 @@
       <c r="D211">
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F211" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>211</v>
       </c>
@@ -4921,8 +6242,11 @@
       <c r="D212">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F212" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>212</v>
       </c>
@@ -4935,8 +6259,11 @@
       <c r="D213">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F213" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>213</v>
       </c>
@@ -4949,8 +6276,11 @@
       <c r="D214">
         <v>0</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F214" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>214</v>
       </c>
@@ -4963,8 +6293,11 @@
       <c r="D215">
         <v>0</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F215" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>215</v>
       </c>
@@ -4977,8 +6310,11 @@
       <c r="D216">
         <v>0</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F216" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>216</v>
       </c>
@@ -4991,8 +6327,11 @@
       <c r="D217">
         <v>0</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F217" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>217</v>
       </c>
@@ -5005,8 +6344,11 @@
       <c r="D218">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F218" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>218</v>
       </c>
@@ -5019,8 +6361,11 @@
       <c r="D219">
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F219" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>219</v>
       </c>
@@ -5033,8 +6378,11 @@
       <c r="D220">
         <v>0</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F220" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>220</v>
       </c>
@@ -5047,8 +6395,11 @@
       <c r="D221">
         <v>0</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F221" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>221</v>
       </c>
@@ -5061,8 +6412,11 @@
       <c r="D222">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F222" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>222</v>
       </c>
@@ -5075,8 +6429,11 @@
       <c r="D223">
         <v>0</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F223" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>223</v>
       </c>
@@ -5089,8 +6446,11 @@
       <c r="D224">
         <v>0</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F224" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>224</v>
       </c>
@@ -5103,8 +6463,11 @@
       <c r="D225">
         <v>0</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F225" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>225</v>
       </c>
@@ -5117,8 +6480,11 @@
       <c r="D226">
         <v>0</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F226" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>226</v>
       </c>
@@ -5131,8 +6497,11 @@
       <c r="D227">
         <v>0</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F227" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>227</v>
       </c>
@@ -5145,8 +6514,11 @@
       <c r="D228">
         <v>0</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F228" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>228</v>
       </c>
@@ -5159,8 +6531,11 @@
       <c r="D229">
         <v>0</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F229" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>229</v>
       </c>
@@ -5173,8 +6548,11 @@
       <c r="D230">
         <v>0</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F230" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>230</v>
       </c>
@@ -5187,8 +6565,11 @@
       <c r="D231">
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F231" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>231</v>
       </c>
@@ -5201,8 +6582,11 @@
       <c r="D232">
         <v>0</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F232" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>232</v>
       </c>
@@ -5215,8 +6599,11 @@
       <c r="D233">
         <v>0</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F233" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>233</v>
       </c>
@@ -5229,8 +6616,11 @@
       <c r="D234">
         <v>0</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F234" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>234</v>
       </c>
@@ -5243,8 +6633,11 @@
       <c r="D235">
         <v>0</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F235" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>235</v>
       </c>
@@ -5257,8 +6650,11 @@
       <c r="D236">
         <v>0</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F236" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>236</v>
       </c>
@@ -5271,8 +6667,14 @@
       <c r="D237">
         <v>0</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E237" t="s">
+        <v>121</v>
+      </c>
+      <c r="F237" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>237</v>
       </c>
@@ -5285,8 +6687,14 @@
       <c r="D238">
         <v>0</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E238" t="s">
+        <v>121</v>
+      </c>
+      <c r="F238" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>238</v>
       </c>
@@ -5299,8 +6707,14 @@
       <c r="D239">
         <v>0</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E239" t="s">
+        <v>120</v>
+      </c>
+      <c r="F239" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>239</v>
       </c>
@@ -5313,8 +6727,14 @@
       <c r="D240">
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E240" t="s">
+        <v>120</v>
+      </c>
+      <c r="F240" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>240</v>
       </c>
@@ -5326,6 +6746,152 @@
       </c>
       <c r="D241">
         <v>0</v>
+      </c>
+      <c r="E241" t="s">
+        <v>120</v>
+      </c>
+      <c r="F241" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242" t="s">
+        <v>238</v>
+      </c>
+      <c r="C242">
+        <v>0</v>
+      </c>
+      <c r="D242">
+        <v>0</v>
+      </c>
+      <c r="E242" t="s">
+        <v>120</v>
+      </c>
+      <c r="F242" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A243">
+        <v>242</v>
+      </c>
+      <c r="B243" t="s">
+        <v>239</v>
+      </c>
+      <c r="C243">
+        <v>0</v>
+      </c>
+      <c r="D243">
+        <v>0</v>
+      </c>
+      <c r="E243" t="s">
+        <v>121</v>
+      </c>
+      <c r="F243" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A244">
+        <v>243</v>
+      </c>
+      <c r="B244" t="s">
+        <v>241</v>
+      </c>
+      <c r="C244">
+        <v>0</v>
+      </c>
+      <c r="D244">
+        <v>58</v>
+      </c>
+      <c r="E244" t="s">
+        <v>121</v>
+      </c>
+      <c r="F244" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A245">
+        <v>244</v>
+      </c>
+      <c r="B245" t="s">
+        <v>240</v>
+      </c>
+      <c r="C245">
+        <v>0</v>
+      </c>
+      <c r="D245">
+        <v>59</v>
+      </c>
+      <c r="E245" t="s">
+        <v>121</v>
+      </c>
+      <c r="F245" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A246">
+        <v>245</v>
+      </c>
+      <c r="B246" t="s">
+        <v>242</v>
+      </c>
+      <c r="C246">
+        <v>0</v>
+      </c>
+      <c r="D246">
+        <v>0</v>
+      </c>
+      <c r="E246" t="s">
+        <v>120</v>
+      </c>
+      <c r="F246" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A247">
+        <v>246</v>
+      </c>
+      <c r="B247" t="s">
+        <v>243</v>
+      </c>
+      <c r="C247">
+        <v>0</v>
+      </c>
+      <c r="D247">
+        <v>0</v>
+      </c>
+      <c r="E247" t="s">
+        <v>120</v>
+      </c>
+      <c r="F247" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A248">
+        <v>247</v>
+      </c>
+      <c r="B248" t="s">
+        <v>244</v>
+      </c>
+      <c r="C248">
+        <v>0</v>
+      </c>
+      <c r="D248">
+        <v>0</v>
+      </c>
+      <c r="E248" t="s">
+        <v>120</v>
+      </c>
+      <c r="F248" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>